<commit_message>
changed : flush logic changed : buffer is a => has a
</commit_message>
<xml_diff>
--- a/test/Fixture/ExcelDataStore/monster.xlsx
+++ b/test/Fixture/ExcelDataStore/monster.xlsx
@@ -22,11 +22,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">x </t>
+    <t>y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>y</t>
+    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -384,10 +384,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>